<commit_message>
python excel into db
</commit_message>
<xml_diff>
--- a/DatabaseInit/XLSDIR/bookInformation.xlsx
+++ b/DatabaseInit/XLSDIR/bookInformation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>bookname</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -28,15 +28,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>d's'f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三方</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dsf</t>
+    <t>毛概</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邓论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旅游</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TP123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TP12324</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A23132</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x213213</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2343232</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1243245</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,12 +413,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -409,36 +434,36 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>3232</v>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>2323</v>
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>4343</v>
-      </c>
-      <c r="B4">
-        <v>43543</v>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>